<commit_message>
Added time series, IG projections, dfs updated w/ correct vals,
</commit_message>
<xml_diff>
--- a/results/GMT_CASE.xlsx
+++ b/results/GMT_CASE.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S109"/>
+  <dimension ref="A1:S112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,22 +379,22 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>layer</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>weight</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -468,21 +468,21 @@
       <c r="C2" t="n">
         <v>8</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -543,21 +543,21 @@
       <c r="C3" t="n">
         <v>19</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -599,7 +599,7 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>1.169621861835507</v>
+        <v>-1.006023548308732</v>
       </c>
       <c r="R3" t="n">
         <v>1</v>
@@ -618,21 +618,21 @@
       <c r="C4" t="n">
         <v>8</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D4" t="n">
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -693,21 +693,21 @@
       <c r="C5" t="n">
         <v>8</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D5" t="n">
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -768,21 +768,21 @@
       <c r="C6" t="n">
         <v>8</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D6" t="n">
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="n">
-        <v>1</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -843,21 +843,21 @@
       <c r="C7" t="n">
         <v>17</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -899,7 +899,7 @@
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>0.2599889880790425</v>
+        <v>-0.04536280397755199</v>
       </c>
       <c r="R7" t="n">
         <v>1</v>
@@ -918,21 +918,21 @@
       <c r="C8" t="n">
         <v>18</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D8" t="n">
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
-      <c r="G8" t="n">
-        <v>1</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>174.259988988079</v>
+        <v>173.9546371960224</v>
       </c>
       <c r="R8" t="n">
         <v>1</v>
@@ -993,21 +993,21 @@
       <c r="C9" t="n">
         <v>17</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D9" t="n">
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
-      <c r="G9" t="n">
-        <v>1</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>0.2599889880790425</v>
+        <v>-0.04536280397755199</v>
       </c>
       <c r="R9" t="n">
         <v>1</v>
@@ -1068,21 +1068,21 @@
       <c r="C10" t="n">
         <v>18</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D10" t="n">
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
-      <c r="G10" t="n">
-        <v>1</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>174.259988988079</v>
+        <v>173.9546371960224</v>
       </c>
       <c r="R10" t="n">
         <v>1</v>
@@ -1143,21 +1143,21 @@
       <c r="C11" t="n">
         <v>19</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D11" t="n">
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
-      <c r="G11" t="n">
-        <v>1</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>1.169621861835507</v>
+        <v>-1.006023548308732</v>
       </c>
       <c r="R11" t="n">
         <v>1</v>
@@ -1218,21 +1218,21 @@
       <c r="C12" t="n">
         <v>21</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D12" t="n">
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
-      <c r="G12" t="n">
-        <v>1</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1293,21 +1293,21 @@
       <c r="C13" t="n">
         <v>21</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D13" t="n">
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
-      <c r="G13" t="n">
-        <v>1</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1368,21 +1368,21 @@
       <c r="C14" t="n">
         <v>15</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D14" t="n">
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
-      <c r="G14" t="n">
-        <v>1</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>43370.02630385487</v>
+        <v>40628</v>
       </c>
       <c r="R14" t="n">
         <v>1</v>
@@ -1443,21 +1443,21 @@
       <c r="C15" t="n">
         <v>31</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D15" t="n">
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
-      <c r="G15" t="n">
-        <v>1</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1499,7 +1499,7 @@
         </is>
       </c>
       <c r="Q15" t="n">
-        <v>9.990011011920958</v>
+        <v>10.29536280397755</v>
       </c>
       <c r="R15" t="n">
         <v>1</v>
@@ -1518,21 +1518,21 @@
       <c r="C16" t="n">
         <v>30</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D16" t="n">
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
-      <c r="G16" t="n">
-        <v>1</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1574,7 +1574,7 @@
         </is>
       </c>
       <c r="Q16" t="n">
-        <v>119.3599927964712</v>
+        <v>117.7615929900561</v>
       </c>
       <c r="R16" t="n">
         <v>1</v>
@@ -1593,21 +1593,21 @@
       <c r="C17" t="n">
         <v>14</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D17" t="n">
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
-      <c r="G17" t="n">
-        <v>1</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1649,7 +1649,7 @@
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="R17" t="n">
         <v>1</v>
@@ -1668,21 +1668,21 @@
       <c r="C18" t="n">
         <v>28</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D18" t="n">
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
-      <c r="G18" t="n">
-        <v>1</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1724,7 +1724,7 @@
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>
@@ -1743,21 +1743,21 @@
       <c r="C19" t="n">
         <v>29</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D19" t="n">
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
-      <c r="G19" t="n">
-        <v>1</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1799,7 +1799,7 @@
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="R19" t="n">
         <v>1</v>
@@ -1818,21 +1818,21 @@
       <c r="C20" t="n">
         <v>14</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D20" t="n">
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
-      <c r="G20" t="n">
-        <v>1</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1849,11 +1849,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K20" t="n">
-        <v>211.5229024943311</v>
-      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
@@ -1874,7 +1872,7 @@
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="R20" t="n">
         <v>1</v>
@@ -1893,21 +1891,21 @@
       <c r="C21" t="n">
         <v>28</v>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D21" t="n">
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
-      <c r="G21" t="n">
-        <v>1</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1924,11 +1922,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K21" t="n">
-        <v>211.5229024943311</v>
-      </c>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -1949,7 +1945,7 @@
         </is>
       </c>
       <c r="Q21" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="R21" t="n">
         <v>1</v>
@@ -1968,21 +1964,21 @@
       <c r="C22" t="n">
         <v>29</v>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D22" t="n">
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
-      <c r="G22" t="n">
-        <v>1</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1999,11 +1995,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K22" t="n">
-        <v>211.5229024943311</v>
-      </c>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
@@ -2024,7 +2018,7 @@
         </is>
       </c>
       <c r="Q22" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="R22" t="n">
         <v>1</v>
@@ -2043,21 +2037,21 @@
       <c r="C23" t="n">
         <v>79</v>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>CREATE</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F23" t="n">
         <v>3</v>
       </c>
-      <c r="G23" t="n">
-        <v>1</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -2074,11 +2068,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K23" t="n">
-        <v>211.5229024943311</v>
-      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
         <v>0</v>
@@ -2098,11 +2090,9 @@
           <t>I_GLOBAL</t>
         </is>
       </c>
-      <c r="Q23" t="n">
-        <v>211.5229024943311</v>
-      </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23" t="n">
         <v>3</v>
@@ -2118,21 +2108,21 @@
       <c r="C24" t="n">
         <v>14</v>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D24" t="n">
+        <v>1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
-      <c r="G24" t="n">
-        <v>1</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -2150,7 +2140,7 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>2530.503401360545</v>
+        <v>0</v>
       </c>
       <c r="L24" t="n">
         <v>1</v>
@@ -2174,7 +2164,7 @@
         </is>
       </c>
       <c r="Q24" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="R24" t="n">
         <v>1</v>
@@ -2193,21 +2183,21 @@
       <c r="C25" t="n">
         <v>28</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D25" t="n">
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
-      <c r="G25" t="n">
-        <v>1</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -2225,7 +2215,7 @@
         </is>
       </c>
       <c r="K25" t="n">
-        <v>2530.503401360545</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
         <v>1</v>
@@ -2249,7 +2239,7 @@
         </is>
       </c>
       <c r="Q25" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="R25" t="n">
         <v>1</v>
@@ -2268,21 +2258,21 @@
       <c r="C26" t="n">
         <v>29</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D26" t="n">
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
-      <c r="G26" t="n">
-        <v>1</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -2300,7 +2290,7 @@
         </is>
       </c>
       <c r="K26" t="n">
-        <v>2530.503401360545</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
         <v>1</v>
@@ -2324,7 +2314,7 @@
         </is>
       </c>
       <c r="Q26" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="R26" t="n">
         <v>1</v>
@@ -2343,21 +2333,21 @@
       <c r="C27" t="n">
         <v>15</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D27" t="n">
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
-      <c r="G27" t="n">
-        <v>1</v>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -2375,7 +2365,7 @@
         </is>
       </c>
       <c r="K27" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="L27" t="n">
         <v>1</v>
@@ -2399,7 +2389,7 @@
         </is>
       </c>
       <c r="Q27" t="n">
-        <v>43370.02630385487</v>
+        <v>40628</v>
       </c>
       <c r="R27" t="n">
         <v>1</v>
@@ -2418,21 +2408,21 @@
       <c r="C28" t="n">
         <v>31</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D28" t="n">
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
-      <c r="G28" t="n">
-        <v>1</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -2450,7 +2440,7 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="L28" t="n">
         <v>1</v>
@@ -2474,7 +2464,7 @@
         </is>
       </c>
       <c r="Q28" t="n">
-        <v>9.990011011920958</v>
+        <v>10.29536280397755</v>
       </c>
       <c r="R28" t="n">
         <v>1</v>
@@ -2493,21 +2483,21 @@
       <c r="C29" t="n">
         <v>30</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D29" t="n">
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
-      <c r="G29" t="n">
-        <v>1</v>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -2525,7 +2515,7 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="L29" t="n">
         <v>1</v>
@@ -2549,7 +2539,7 @@
         </is>
       </c>
       <c r="Q29" t="n">
-        <v>119.3599927964712</v>
+        <v>117.7615929900561</v>
       </c>
       <c r="R29" t="n">
         <v>1</v>
@@ -2568,21 +2558,21 @@
       <c r="C30" t="n">
         <v>28</v>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D30" t="n">
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
-      <c r="G30" t="n">
-        <v>1</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -2600,7 +2590,7 @@
         </is>
       </c>
       <c r="K30" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="L30" t="n">
         <v>1</v>
@@ -2624,7 +2614,7 @@
         </is>
       </c>
       <c r="Q30" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="R30" t="n">
         <v>1</v>
@@ -2643,21 +2633,21 @@
       <c r="C31" t="n">
         <v>29</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D31" t="n">
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
-      <c r="G31" t="n">
-        <v>1</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2675,7 +2665,7 @@
         </is>
       </c>
       <c r="K31" t="n">
-        <v>14742.02630385488</v>
+        <v>12000</v>
       </c>
       <c r="L31" t="n">
         <v>1</v>
@@ -2699,7 +2689,7 @@
         </is>
       </c>
       <c r="Q31" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="R31" t="n">
         <v>1</v>
@@ -2718,21 +2708,21 @@
       <c r="C32" t="n">
         <v>16</v>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D32" t="n">
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
-      <c r="G32" t="n">
-        <v>1</v>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -2750,7 +2740,7 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>43370.02630385487</v>
+        <v>40628</v>
       </c>
       <c r="L32" t="n">
         <v>1</v>
@@ -2774,7 +2764,7 @@
         </is>
       </c>
       <c r="Q32" t="n">
-        <v>2.557776395179524</v>
+        <v>-3.926335894036524</v>
       </c>
       <c r="R32" t="n">
         <v>1</v>
@@ -2793,21 +2783,21 @@
       <c r="C33" t="n">
         <v>31</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D33" t="n">
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
-      <c r="G33" t="n">
-        <v>1</v>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -2825,7 +2815,7 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>43370.02630385487</v>
+        <v>40628</v>
       </c>
       <c r="L33" t="n">
         <v>1</v>
@@ -2849,7 +2839,7 @@
         </is>
       </c>
       <c r="Q33" t="n">
-        <v>9.990011011920958</v>
+        <v>10.29536280397755</v>
       </c>
       <c r="R33" t="n">
         <v>1</v>
@@ -2868,21 +2858,21 @@
       <c r="C34" t="n">
         <v>30</v>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D34" t="n">
+        <v>1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="n">
-        <v>1</v>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -2900,7 +2890,7 @@
         </is>
       </c>
       <c r="K34" t="n">
-        <v>43370.02630385487</v>
+        <v>40628</v>
       </c>
       <c r="L34" t="n">
         <v>1</v>
@@ -2924,7 +2914,7 @@
         </is>
       </c>
       <c r="Q34" t="n">
-        <v>119.3599927964712</v>
+        <v>117.7615929900561</v>
       </c>
       <c r="R34" t="n">
         <v>1</v>
@@ -2943,21 +2933,21 @@
       <c r="C35" t="n">
         <v>78</v>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>UPDATE</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F35" t="n">
         <v>7</v>
       </c>
-      <c r="G35" t="n">
-        <v>1</v>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -3018,21 +3008,21 @@
       <c r="C36" t="n">
         <v>19</v>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D36" t="n">
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
-      <c r="G36" t="n">
-        <v>1</v>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -3050,7 +3040,7 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>174.259988988079</v>
+        <v>173.9546371960224</v>
       </c>
       <c r="L36" t="n">
         <v>1</v>
@@ -3074,7 +3064,7 @@
         </is>
       </c>
       <c r="Q36" t="n">
-        <v>1.169621861835507</v>
+        <v>-1.006023548308732</v>
       </c>
       <c r="R36" t="n">
         <v>1</v>
@@ -3093,21 +3083,21 @@
       <c r="C37" t="n">
         <v>13</v>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D37" t="n">
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
-      <c r="G37" t="n">
-        <v>1</v>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -3149,7 +3139,7 @@
         </is>
       </c>
       <c r="Q37" t="n">
-        <v>2530.503401360545</v>
+        <v>0</v>
       </c>
       <c r="R37" t="n">
         <v>1</v>
@@ -3168,21 +3158,21 @@
       <c r="C38" t="n">
         <v>16</v>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D38" t="n">
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F38" t="n">
         <v>0</v>
       </c>
-      <c r="G38" t="n">
-        <v>1</v>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -3224,7 +3214,7 @@
         </is>
       </c>
       <c r="Q38" t="n">
-        <v>2.557776395179524</v>
+        <v>-3.926335894036524</v>
       </c>
       <c r="R38" t="n">
         <v>1</v>
@@ -3243,21 +3233,21 @@
       <c r="C39" t="n">
         <v>28</v>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D39" t="n">
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
-      <c r="G39" t="n">
-        <v>1</v>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -3299,7 +3289,7 @@
         </is>
       </c>
       <c r="Q39" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="R39" t="n">
         <v>1</v>
@@ -3318,21 +3308,21 @@
       <c r="C40" t="n">
         <v>29</v>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D40" t="n">
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F40" t="n">
         <v>0</v>
       </c>
-      <c r="G40" t="n">
-        <v>1</v>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -3374,7 +3364,7 @@
         </is>
       </c>
       <c r="Q40" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="R40" t="n">
         <v>1</v>
@@ -3393,21 +3383,21 @@
       <c r="C41" t="n">
         <v>28</v>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D41" t="n">
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F41" t="n">
         <v>0</v>
       </c>
-      <c r="G41" t="n">
-        <v>1</v>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -3447,7 +3437,7 @@
         </is>
       </c>
       <c r="Q41" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="R41" t="n">
         <v>1</v>
@@ -3466,21 +3456,21 @@
       <c r="C42" t="n">
         <v>29</v>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D42" t="n">
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F42" t="n">
         <v>0</v>
       </c>
-      <c r="G42" t="n">
-        <v>1</v>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -3497,11 +3487,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K42" t="n">
-        <v>23</v>
-      </c>
+      <c r="K42" t="inlineStr"/>
       <c r="L42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
@@ -3522,7 +3510,7 @@
         </is>
       </c>
       <c r="Q42" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="R42" t="n">
         <v>1</v>
@@ -3541,21 +3529,21 @@
       <c r="C43" t="n">
         <v>80</v>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>CREATE</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F43" t="n">
         <v>3</v>
       </c>
-      <c r="G43" t="n">
-        <v>1</v>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -3572,11 +3560,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K43" t="n">
-        <v>23</v>
-      </c>
+      <c r="K43" t="inlineStr"/>
       <c r="L43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" t="n">
         <v>0</v>
@@ -3596,11 +3582,9 @@
           <t>I_GLOBAL</t>
         </is>
       </c>
-      <c r="Q43" t="n">
-        <v>23</v>
-      </c>
+      <c r="Q43" t="inlineStr"/>
       <c r="R43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S43" t="n">
         <v>3</v>
@@ -3616,21 +3600,21 @@
       <c r="C44" t="n">
         <v>28</v>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D44" t="n">
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F44" t="n">
         <v>0</v>
       </c>
-      <c r="G44" t="n">
-        <v>1</v>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -3672,7 +3656,7 @@
         </is>
       </c>
       <c r="Q44" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="R44" t="n">
         <v>1</v>
@@ -3691,21 +3675,21 @@
       <c r="C45" t="n">
         <v>29</v>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D45" t="n">
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
-      <c r="G45" t="n">
-        <v>1</v>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -3747,7 +3731,7 @@
         </is>
       </c>
       <c r="Q45" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="R45" t="n">
         <v>1</v>
@@ -3766,21 +3750,21 @@
       <c r="C46" t="n">
         <v>30</v>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D46" t="n">
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
-      <c r="G46" t="n">
-        <v>1</v>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -3798,7 +3782,7 @@
         </is>
       </c>
       <c r="K46" t="n">
-        <v>121.0300395912554</v>
+        <v>116</v>
       </c>
       <c r="L46" t="n">
         <v>1</v>
@@ -3822,7 +3806,7 @@
         </is>
       </c>
       <c r="Q46" t="n">
-        <v>119.3599927964712</v>
+        <v>117.7615929900561</v>
       </c>
       <c r="R46" t="n">
         <v>1</v>
@@ -3841,21 +3825,21 @@
       <c r="C47" t="n">
         <v>31</v>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D47" t="n">
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F47" t="n">
         <v>0</v>
       </c>
-      <c r="G47" t="n">
-        <v>1</v>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -3873,7 +3857,7 @@
         </is>
       </c>
       <c r="K47" t="n">
-        <v>9.970613084876691</v>
+        <v>11</v>
       </c>
       <c r="L47" t="n">
         <v>1</v>
@@ -3897,7 +3881,7 @@
         </is>
       </c>
       <c r="Q47" t="n">
-        <v>9.990011011920958</v>
+        <v>10.29536280397755</v>
       </c>
       <c r="R47" t="n">
         <v>1</v>
@@ -3916,21 +3900,21 @@
       <c r="C48" t="n">
         <v>19</v>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D48" t="n">
+        <v>1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F48" t="n">
         <v>0</v>
       </c>
-      <c r="G48" t="n">
-        <v>1</v>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -3948,7 +3932,7 @@
         </is>
       </c>
       <c r="K48" t="n">
-        <v>119.3599927964712</v>
+        <v>117.7615929900561</v>
       </c>
       <c r="L48" t="n">
         <v>1</v>
@@ -3972,7 +3956,7 @@
         </is>
       </c>
       <c r="Q48" t="n">
-        <v>1.169621861835507</v>
+        <v>-1.006023548308732</v>
       </c>
       <c r="R48" t="n">
         <v>1</v>
@@ -3991,21 +3975,21 @@
       <c r="C49" t="n">
         <v>17</v>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D49" t="n">
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F49" t="n">
         <v>0</v>
       </c>
-      <c r="G49" t="n">
-        <v>1</v>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
@@ -4023,7 +4007,7 @@
         </is>
       </c>
       <c r="K49" t="n">
-        <v>9.990011011920958</v>
+        <v>10.29536280397755</v>
       </c>
       <c r="L49" t="n">
         <v>1</v>
@@ -4047,7 +4031,7 @@
         </is>
       </c>
       <c r="Q49" t="n">
-        <v>0.2599889880790425</v>
+        <v>-0.04536280397755199</v>
       </c>
       <c r="R49" t="n">
         <v>1</v>
@@ -4066,21 +4050,21 @@
       <c r="C50" t="n">
         <v>18</v>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D50" t="n">
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F50" t="n">
         <v>0</v>
       </c>
-      <c r="G50" t="n">
-        <v>1</v>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -4098,7 +4082,7 @@
         </is>
       </c>
       <c r="K50" t="n">
-        <v>9.990011011920958</v>
+        <v>10.29536280397755</v>
       </c>
       <c r="L50" t="n">
         <v>1</v>
@@ -4122,7 +4106,7 @@
         </is>
       </c>
       <c r="Q50" t="n">
-        <v>174.259988988079</v>
+        <v>173.9546371960224</v>
       </c>
       <c r="R50" t="n">
         <v>1</v>
@@ -4141,21 +4125,21 @@
       <c r="C51" t="n">
         <v>30</v>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D51" t="n">
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="n">
-        <v>1</v>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -4197,7 +4181,7 @@
         </is>
       </c>
       <c r="Q51" t="n">
-        <v>119.3599927964712</v>
+        <v>117.7615929900561</v>
       </c>
       <c r="R51" t="n">
         <v>1</v>
@@ -4216,21 +4200,21 @@
       <c r="C52" t="n">
         <v>31</v>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D52" t="n">
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="n">
-        <v>1</v>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -4272,7 +4256,7 @@
         </is>
       </c>
       <c r="Q52" t="n">
-        <v>9.990011011920958</v>
+        <v>10.29536280397755</v>
       </c>
       <c r="R52" t="n">
         <v>1</v>
@@ -4291,21 +4275,21 @@
       <c r="C53" t="n">
         <v>13</v>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D53" t="n">
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="F53" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="n">
-        <v>1</v>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -4322,11 +4306,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K53" t="n">
-        <v>2994.678581491768</v>
-      </c>
+      <c r="K53" t="inlineStr"/>
       <c r="L53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M53" t="n">
         <v>0</v>
@@ -4347,7 +4329,7 @@
         </is>
       </c>
       <c r="Q53" t="n">
-        <v>2530.503401360545</v>
+        <v>0</v>
       </c>
       <c r="R53" t="n">
         <v>1</v>
@@ -4366,21 +4348,21 @@
       <c r="C54" t="n">
         <v>81</v>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>CREATE</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F54" t="n">
         <v>3</v>
       </c>
-      <c r="G54" t="n">
-        <v>1</v>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -4397,11 +4379,9 @@
           <t>NAVARCH</t>
         </is>
       </c>
-      <c r="K54" t="n">
-        <v>2994.678581491768</v>
-      </c>
+      <c r="K54" t="inlineStr"/>
       <c r="L54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54" t="n">
         <v>0</v>
@@ -4421,11 +4401,9 @@
           <t>I_GLOBAL</t>
         </is>
       </c>
-      <c r="Q54" t="n">
-        <v>2994.678581491768</v>
-      </c>
+      <c r="Q54" t="inlineStr"/>
       <c r="R54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S54" t="n">
         <v>3</v>
@@ -4441,21 +4419,21 @@
       <c r="C55" t="n">
         <v>47</v>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D55" t="n">
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>1</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -4516,21 +4494,21 @@
       <c r="C56" t="n">
         <v>47</v>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D56" t="n">
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>1</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -4591,21 +4569,21 @@
       <c r="C57" t="n">
         <v>47</v>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D57" t="n">
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="n">
-        <v>1</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -4666,21 +4644,21 @@
       <c r="C58" t="n">
         <v>47</v>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D58" t="n">
+        <v>1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
-        <v>1</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -4741,21 +4719,21 @@
       <c r="C59" t="n">
         <v>35</v>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D59" t="n">
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
-        <v>1</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
@@ -4816,21 +4794,21 @@
       <c r="C60" t="n">
         <v>55</v>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D60" t="n">
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="n">
-        <v>1</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
@@ -4891,21 +4869,21 @@
       <c r="C61" t="n">
         <v>36</v>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D61" t="n">
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F61" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="n">
-        <v>1</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -4966,21 +4944,21 @@
       <c r="C62" t="n">
         <v>55</v>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D62" t="n">
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="n">
-        <v>1</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -5041,21 +5019,21 @@
       <c r="C63" t="n">
         <v>37</v>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D63" t="n">
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="n">
-        <v>1</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
@@ -5116,21 +5094,21 @@
       <c r="C64" t="n">
         <v>55</v>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D64" t="n">
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="n">
-        <v>1</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -5191,21 +5169,21 @@
       <c r="C65" t="n">
         <v>38</v>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D65" t="n">
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F65" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="n">
-        <v>1</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
@@ -5266,21 +5244,21 @@
       <c r="C66" t="n">
         <v>55</v>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D66" t="n">
+        <v>1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F66" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" t="n">
-        <v>1</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -5341,21 +5319,21 @@
       <c r="C67" t="n">
         <v>35</v>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D67" t="n">
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F67" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" t="n">
-        <v>1</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -5416,21 +5394,21 @@
       <c r="C68" t="n">
         <v>36</v>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D68" t="n">
+        <v>1</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="n">
-        <v>1</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
@@ -5491,21 +5469,21 @@
       <c r="C69" t="n">
         <v>37</v>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D69" t="n">
+        <v>1</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="n">
-        <v>1</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
@@ -5566,21 +5544,21 @@
       <c r="C70" t="n">
         <v>38</v>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D70" t="n">
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="n">
-        <v>1</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -5641,21 +5619,21 @@
       <c r="C71" t="n">
         <v>79</v>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="inlineStr">
         <is>
           <t>UPDATE</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F71" t="n">
         <v>5</v>
       </c>
-      <c r="G71" t="n">
-        <v>1</v>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -5716,21 +5694,21 @@
       <c r="C72" t="n">
         <v>80</v>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>UPDATE</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F72" t="n">
         <v>5</v>
       </c>
-      <c r="G72" t="n">
-        <v>1</v>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -5791,21 +5769,21 @@
       <c r="C73" t="n">
         <v>55</v>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D73" t="n">
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F73" t="n">
-        <v>0</v>
-      </c>
-      <c r="G73" t="n">
-        <v>1</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
@@ -5866,21 +5844,21 @@
       <c r="C74" t="n">
         <v>55</v>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D74" t="n">
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F74" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="n">
-        <v>1</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
@@ -5941,21 +5919,21 @@
       <c r="C75" t="n">
         <v>61</v>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D75" t="n">
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F75" t="n">
-        <v>0</v>
-      </c>
-      <c r="G75" t="n">
-        <v>1</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
@@ -6016,21 +5994,21 @@
       <c r="C76" t="n">
         <v>61</v>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D76" t="n">
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F76" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" t="n">
-        <v>1</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
@@ -6091,21 +6069,21 @@
       <c r="C77" t="n">
         <v>55</v>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D77" t="n">
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F77" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" t="n">
-        <v>1</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
@@ -6166,21 +6144,21 @@
       <c r="C78" t="n">
         <v>81</v>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" t="inlineStr">
         <is>
           <t>UPDATE</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F78" t="n">
         <v>5</v>
       </c>
-      <c r="G78" t="n">
-        <v>1</v>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
@@ -6241,21 +6219,21 @@
       <c r="C79" t="n">
         <v>55</v>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D79" t="n">
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F79" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" t="n">
-        <v>1</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
@@ -6316,21 +6294,21 @@
       <c r="C80" t="n">
         <v>55</v>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D80" t="n">
+        <v>1</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F80" t="n">
-        <v>0</v>
-      </c>
-      <c r="G80" t="n">
-        <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
@@ -6391,21 +6369,21 @@
       <c r="C81" t="n">
         <v>55</v>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D81" t="n">
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F81" t="n">
-        <v>0</v>
-      </c>
-      <c r="G81" t="n">
-        <v>1</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
@@ -6466,21 +6444,21 @@
       <c r="C82" t="n">
         <v>55</v>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D82" t="n">
+        <v>1</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F82" t="n">
-        <v>0</v>
-      </c>
-      <c r="G82" t="n">
-        <v>1</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
@@ -6541,21 +6519,21 @@
       <c r="C83" t="n">
         <v>55</v>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D83" t="n">
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F83" t="n">
-        <v>0</v>
-      </c>
-      <c r="G83" t="n">
-        <v>1</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
@@ -6616,21 +6594,21 @@
       <c r="C84" t="n">
         <v>61</v>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D84" t="n">
+        <v>1</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
-      </c>
-      <c r="F84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" t="n">
-        <v>1</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
@@ -6691,21 +6669,21 @@
       <c r="C85" t="n">
         <v>67</v>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D85" t="n">
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F85" t="n">
-        <v>0</v>
-      </c>
-      <c r="G85" t="n">
-        <v>1</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
@@ -6766,21 +6744,21 @@
       <c r="C86" t="n">
         <v>67</v>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D86" t="n">
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F86" t="n">
-        <v>0</v>
-      </c>
-      <c r="G86" t="n">
-        <v>1</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
@@ -6841,21 +6819,21 @@
       <c r="C87" t="n">
         <v>66</v>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D87" t="n">
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F87" t="n">
-        <v>0</v>
-      </c>
-      <c r="G87" t="n">
-        <v>1</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
@@ -6916,21 +6894,21 @@
       <c r="C88" t="n">
         <v>66</v>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D88" t="n">
+        <v>1</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F88" t="n">
-        <v>0</v>
-      </c>
-      <c r="G88" t="n">
-        <v>1</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
@@ -6989,21 +6967,21 @@
       <c r="C89" t="n">
         <v>76</v>
       </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D89" t="n">
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F89" t="n">
-        <v>0</v>
-      </c>
-      <c r="G89" t="n">
-        <v>1</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
@@ -7062,21 +7040,21 @@
       <c r="C90" t="n">
         <v>74</v>
       </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D90" t="n">
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G90" t="n">
-        <v>1</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
@@ -7137,21 +7115,21 @@
       <c r="C91" t="n">
         <v>75</v>
       </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D91" t="n">
+        <v>1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F91" t="n">
-        <v>0</v>
-      </c>
-      <c r="G91" t="n">
-        <v>1</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
@@ -7212,21 +7190,21 @@
       <c r="C92" t="n">
         <v>76</v>
       </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D92" t="n">
+        <v>1</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G92" t="n">
-        <v>1</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
@@ -7287,21 +7265,21 @@
       <c r="C93" t="n">
         <v>66</v>
       </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D93" t="n">
+        <v>1</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F93" t="n">
-        <v>0</v>
-      </c>
-      <c r="G93" t="n">
-        <v>1</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
@@ -7362,21 +7340,21 @@
       <c r="C94" t="n">
         <v>75</v>
       </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D94" t="n">
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F94" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="n">
-        <v>1</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
@@ -7437,21 +7415,21 @@
       <c r="C95" t="n">
         <v>75</v>
       </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D95" t="n">
+        <v>1</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F95" t="n">
-        <v>0</v>
-      </c>
-      <c r="G95" t="n">
-        <v>1</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
@@ -7512,22 +7490,22 @@
       <c r="C96" t="n">
         <v>75</v>
       </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D96" t="n">
+        <v>1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
       </c>
-      <c r="F96" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="n">
-        <v>1</v>
-      </c>
       <c r="H96" t="inlineStr">
         <is>
           <t>(-190.0961, 754.6295, 0.0)</t>
@@ -7535,7 +7513,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>Z1</t>
+          <t>z_fuel</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -7585,22 +7563,22 @@
       <c r="C97" t="n">
         <v>75</v>
       </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D97" t="n">
+        <v>1</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
       </c>
-      <c r="F97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G97" t="n">
-        <v>1</v>
-      </c>
       <c r="H97" t="inlineStr">
         <is>
           <t>(-229.1853, 488.39224, 0.0)</t>
@@ -7608,7 +7586,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>Z2</t>
+          <t>z_veh</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -7658,21 +7636,21 @@
       <c r="C98" t="n">
         <v>75</v>
       </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D98" t="n">
+        <v>1</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F98" t="n">
-        <v>0</v>
-      </c>
-      <c r="G98" t="n">
-        <v>1</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
@@ -7733,21 +7711,21 @@
       <c r="C99" t="n">
         <v>75</v>
       </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D99" t="n">
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F99" t="n">
-        <v>0</v>
-      </c>
-      <c r="G99" t="n">
-        <v>1</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
@@ -7808,21 +7786,21 @@
       <c r="C100" t="n">
         <v>76</v>
       </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>INTERNAL</t>
-        </is>
+      <c r="D100" t="n">
+        <v>1</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
+          <t>INTERNAL</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
           <t>DIST</t>
         </is>
-      </c>
-      <c r="F100" t="n">
-        <v>0</v>
-      </c>
-      <c r="G100" t="n">
-        <v>1</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
@@ -7883,22 +7861,22 @@
       <c r="C101" t="n">
         <v>78</v>
       </c>
-      <c r="D101" t="inlineStr">
+      <c r="D101" t="n">
+        <v>1</v>
+      </c>
+      <c r="E101" t="inlineStr">
         <is>
           <t>CREATE</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr">
+      <c r="F101" t="n">
+        <v>1</v>
+      </c>
+      <c r="G101" t="inlineStr">
         <is>
           <t>BETWEEN</t>
         </is>
       </c>
-      <c r="F101" t="n">
-        <v>1</v>
-      </c>
-      <c r="G101" t="n">
-        <v>1</v>
-      </c>
       <c r="H101" t="inlineStr">
         <is>
           <t>(0.0, 0.0, 0.0)</t>
@@ -7914,11 +7892,9 @@
           <t>K_GLOBAL</t>
         </is>
       </c>
-      <c r="K101" t="n">
-        <v>0.2599889880790425</v>
-      </c>
+      <c r="K101" t="inlineStr"/>
       <c r="L101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M101" t="n">
         <v>1</v>
@@ -7938,11 +7914,9 @@
           <t>I_GLOBAL</t>
         </is>
       </c>
-      <c r="Q101" t="n">
-        <v>0.2599889880790425</v>
-      </c>
+      <c r="Q101" t="inlineStr"/>
       <c r="R101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S101" t="n">
         <v>1</v>
@@ -7958,21 +7932,21 @@
       <c r="C102" t="n">
         <v>17</v>
       </c>
-      <c r="D102" t="inlineStr">
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" t="inlineStr">
         <is>
           <t>SELECT</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F102" t="n">
         <v>2</v>
       </c>
-      <c r="G102" t="n">
-        <v>1</v>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
@@ -7989,11 +7963,9 @@
           <t>I_GLOBAL</t>
         </is>
       </c>
-      <c r="K102" t="n">
-        <v>0.2599889880790425</v>
-      </c>
+      <c r="K102" t="inlineStr"/>
       <c r="L102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M102" t="n">
         <v>1</v>
@@ -8014,7 +7986,7 @@
         </is>
       </c>
       <c r="Q102" t="n">
-        <v>0.2599889880790425</v>
+        <v>-0.04536280397755199</v>
       </c>
       <c r="R102" t="n">
         <v>1</v>
@@ -8033,21 +8005,21 @@
       <c r="C103" t="n">
         <v>77</v>
       </c>
-      <c r="D103" t="inlineStr">
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" t="inlineStr">
         <is>
           <t>UPDATE</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F103" t="n">
         <v>8</v>
       </c>
-      <c r="G103" t="n">
-        <v>1</v>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
@@ -8108,21 +8080,21 @@
       <c r="C104" t="n">
         <v>47</v>
       </c>
-      <c r="D104" t="inlineStr">
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="inlineStr">
         <is>
           <t>SELECT</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F104" t="n">
         <v>4</v>
       </c>
-      <c r="G104" t="n">
-        <v>1</v>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
@@ -8139,11 +8111,9 @@
           <t>I_GLOBAL</t>
         </is>
       </c>
-      <c r="K104" t="n">
-        <v>211.5229024943311</v>
-      </c>
+      <c r="K104" t="inlineStr"/>
       <c r="L104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M104" t="n">
         <v>3</v>
@@ -8183,21 +8153,21 @@
       <c r="C105" t="n">
         <v>12</v>
       </c>
-      <c r="D105" t="inlineStr">
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="inlineStr">
         <is>
           <t>UPDATE</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>BETWEEN</t>
         </is>
       </c>
       <c r="F105" t="n">
         <v>6</v>
       </c>
-      <c r="G105" t="n">
-        <v>1</v>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
@@ -8253,26 +8223,26 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C106" t="n">
-        <v>49</v>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>SELECT</t>
-        </is>
+        <v>78</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>BETWEEN</t>
+          <t>PROJECTION</t>
         </is>
       </c>
       <c r="F106" t="n">
-        <v>4</v>
-      </c>
-      <c r="G106" t="n">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
@@ -8281,7 +8251,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>z_veh</t>
+          <t>W_veh</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -8290,7 +8260,7 @@
         </is>
       </c>
       <c r="K106" t="n">
-        <v>23</v>
+        <v>211.5229024943311</v>
       </c>
       <c r="L106" t="n">
         <v>1</v>
@@ -8300,27 +8270,27 @@
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>(360.91547, -500.96497, 0.0)</t>
+          <t>(0.0, 0.0, 0.0)</t>
         </is>
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>z_veh</t>
+          <t>GMT</t>
         </is>
       </c>
       <c r="P106" t="inlineStr">
         <is>
-          <t>OPS</t>
+          <t>I_GLOBAL</t>
         </is>
       </c>
       <c r="Q106" t="n">
-        <v>23</v>
+        <v>0.2599889880790425</v>
       </c>
       <c r="R106" t="n">
         <v>1</v>
       </c>
       <c r="S106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -8331,24 +8301,24 @@
         <v>80</v>
       </c>
       <c r="C107" t="n">
-        <v>25</v>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>UPDATE</t>
-        </is>
+        <v>49</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
+          <t>SELECT</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>4</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
           <t>BETWEEN</t>
         </is>
       </c>
-      <c r="F107" t="n">
-        <v>6</v>
-      </c>
-      <c r="G107" t="n">
-        <v>1</v>
-      </c>
       <c r="H107" t="inlineStr">
         <is>
           <t>(0.0, 0.0, 0.0)</t>
@@ -8364,18 +8334,16 @@
           <t>I_GLOBAL</t>
         </is>
       </c>
-      <c r="K107" t="n">
-        <v>23</v>
-      </c>
+      <c r="K107" t="inlineStr"/>
       <c r="L107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M107" t="n">
         <v>3</v>
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>(398.22684, 18.430798, 0.0)</t>
+          <t>(360.91547, -500.96497, 0.0)</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -8385,7 +8353,7 @@
       </c>
       <c r="P107" t="inlineStr">
         <is>
-          <t>NAVARCH</t>
+          <t>OPS</t>
         </is>
       </c>
       <c r="Q107" t="n">
@@ -8403,27 +8371,27 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C108" t="n">
-        <v>55</v>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>SELECT</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
+          <t>UPDATE</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>6</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
           <t>BETWEEN</t>
         </is>
       </c>
-      <c r="F108" t="n">
-        <v>4</v>
-      </c>
-      <c r="G108" t="n">
-        <v>1</v>
-      </c>
       <c r="H108" t="inlineStr">
         <is>
           <t>(0.0, 0.0, 0.0)</t>
@@ -8431,7 +8399,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>V_fuel</t>
+          <t>z_veh</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
@@ -8440,7 +8408,7 @@
         </is>
       </c>
       <c r="K108" t="n">
-        <v>2994.678581491768</v>
+        <v>23</v>
       </c>
       <c r="L108" t="n">
         <v>1</v>
@@ -8450,21 +8418,21 @@
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>(145.98741, -112.20771, 0.0)</t>
+          <t>(398.22684, 18.430798, 0.0)</t>
         </is>
       </c>
       <c r="O108" t="inlineStr">
         <is>
-          <t>V_fuel</t>
+          <t>z_veh</t>
         </is>
       </c>
       <c r="P108" t="inlineStr">
         <is>
-          <t>OPS</t>
+          <t>NAVARCH</t>
         </is>
       </c>
       <c r="Q108" t="n">
-        <v>2994.678581491768</v>
+        <v>23</v>
       </c>
       <c r="R108" t="n">
         <v>1</v>
@@ -8478,26 +8446,26 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C109" t="n">
-        <v>34</v>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>UPDATE</t>
-        </is>
+        <v>78</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>BETWEEN</t>
+          <t>PROJECTION</t>
         </is>
       </c>
       <c r="F109" t="n">
-        <v>6</v>
-      </c>
-      <c r="G109" t="n">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
       </c>
       <c r="H109" t="inlineStr">
         <is>
@@ -8506,7 +8474,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>V_fuel</t>
+          <t>z_veh</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
@@ -8515,7 +8483,7 @@
         </is>
       </c>
       <c r="K109" t="n">
-        <v>2994.678581491768</v>
+        <v>23</v>
       </c>
       <c r="L109" t="n">
         <v>1</v>
@@ -8525,27 +8493,250 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
+          <t>(0.0, 0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>GMT</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
+      </c>
+      <c r="Q109" t="n">
+        <v>0.2599889880790425</v>
+      </c>
+      <c r="R109" t="n">
+        <v>1</v>
+      </c>
+      <c r="S109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>81</v>
+      </c>
+      <c r="C110" t="n">
+        <v>55</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>SELECT</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>4</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>V_fuel</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M110" t="n">
+        <v>3</v>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>(145.98741, -112.20771, 0.0)</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>V_fuel</t>
+        </is>
+      </c>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+      <c r="Q110" t="n">
+        <v>2994.678581491768</v>
+      </c>
+      <c r="R110" t="n">
+        <v>1</v>
+      </c>
+      <c r="S110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>81</v>
+      </c>
+      <c r="C111" t="n">
+        <v>34</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>UPDATE</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>6</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>BETWEEN</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>V_fuel</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
+      </c>
+      <c r="K111" t="n">
+        <v>2994.678581491768</v>
+      </c>
+      <c r="L111" t="n">
+        <v>1</v>
+      </c>
+      <c r="M111" t="n">
+        <v>3</v>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
           <t>(686.00525, 388.09482, 0.0)</t>
         </is>
       </c>
-      <c r="O109" t="inlineStr">
+      <c r="O111" t="inlineStr">
         <is>
           <t>V_fuel</t>
         </is>
       </c>
-      <c r="P109" t="inlineStr">
-        <is>
-          <t>NAVARCH</t>
-        </is>
-      </c>
-      <c r="Q109" t="n">
+      <c r="P111" t="inlineStr">
+        <is>
+          <t>NAVARCH</t>
+        </is>
+      </c>
+      <c r="Q111" t="n">
         <v>2994.678581491768</v>
       </c>
-      <c r="R109" t="n">
-        <v>1</v>
-      </c>
-      <c r="S109" t="n">
-        <v>0</v>
+      <c r="R111" t="n">
+        <v>1</v>
+      </c>
+      <c r="S111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>81</v>
+      </c>
+      <c r="C112" t="n">
+        <v>78</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>PROJECTION</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>7</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>V_fuel</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
+      </c>
+      <c r="K112" t="n">
+        <v>2994.678581491768</v>
+      </c>
+      <c r="L112" t="n">
+        <v>1</v>
+      </c>
+      <c r="M112" t="n">
+        <v>3</v>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>GMT</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>I_GLOBAL</t>
+        </is>
+      </c>
+      <c r="Q112" t="n">
+        <v>0.2599889880790425</v>
+      </c>
+      <c r="R112" t="n">
+        <v>1</v>
+      </c>
+      <c r="S112" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>